<commit_message>
Edited the File Controller and Updated the REGISTER FILE.
</commit_message>
<xml_diff>
--- a/Classistant_JSON_Format.xlsx
+++ b/Classistant_JSON_Format.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28315"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pronoymukherjee/OneDrive/Android/Classistant/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10935"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="10940"/>
   </bookViews>
   <sheets>
     <sheet name="Queries_JSON" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>class:</t>
   </si>
@@ -198,12 +204,15 @@
   </si>
   <si>
     <t>total number of class held by the teacher</t>
+  </si>
+  <si>
+    <t>insert into StudentMetadata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -572,21 +581,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
@@ -594,7 +603,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
@@ -604,7 +613,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -614,7 +623,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -624,7 +633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
@@ -634,18 +643,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" t="s">
@@ -655,7 +664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" t="s">
@@ -665,7 +674,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
@@ -675,21 +684,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="2" t="s">
@@ -699,7 +708,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" t="s">
@@ -709,7 +718,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
@@ -719,7 +728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" t="s">
@@ -729,7 +738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" t="s">
@@ -739,7 +748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
@@ -749,7 +758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" t="s">
@@ -759,7 +768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" t="s">
@@ -769,11 +778,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>45</v>
@@ -785,17 +794,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
@@ -805,7 +814,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" t="s">
@@ -815,7 +824,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" t="s">
@@ -825,7 +834,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
@@ -835,7 +844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" t="s">
@@ -845,7 +854,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" t="s">
@@ -855,7 +864,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
@@ -865,7 +874,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" t="s">
@@ -875,7 +884,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" t="s">
@@ -885,7 +894,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
@@ -895,11 +904,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
         <v>42</v>
@@ -911,7 +920,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" t="s">
@@ -921,7 +930,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" t="s">
@@ -931,7 +940,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" t="s">
@@ -941,11 +950,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="3" t="s">
         <v>48</v>
@@ -957,7 +966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" t="s">
@@ -967,7 +976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" t="s">
@@ -977,7 +986,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" t="s">
@@ -987,7 +996,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" t="s">
@@ -997,7 +1006,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" t="s">
@@ -1007,7 +1016,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" t="s">

</xml_diff>